<commit_message>
Demo stats for manuscript
</commit_message>
<xml_diff>
--- a/tables/SART-Ppt-Demo-Questionnaire-Scores.xlsx
+++ b/tables/SART-Ppt-Demo-Questionnaire-Scores.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/elaine/Desktop/Git_Studies/MWMB_ADHD/tables/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0DDE504C-88BB-3247-B79A-1F6B428FE925}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9CA154A8-0587-1446-B84B-B17F17BF0EB6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16080" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="361" uniqueCount="101">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="424" uniqueCount="105">
   <si>
     <t>SubID</t>
   </si>
@@ -337,12 +337,24 @@
   <si>
     <t>C044</t>
   </si>
+  <si>
+    <t>may be excessively sleepy</t>
+  </si>
+  <si>
+    <t>unlikely to be abnormally sleepy.</t>
+  </si>
+  <si>
+    <t>average amount of daytime sleepiness.</t>
+  </si>
+  <si>
+    <t>excessively sleepy.</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -363,6 +375,11 @@
       <name val="Arial"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF434343"/>
+      <name val="Roboto"/>
     </font>
   </fonts>
   <fills count="2">
@@ -535,7 +552,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -582,19 +599,12 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="35">
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFCC4125"/>
-          <bgColor rgb="FFCC4125"/>
-        </patternFill>
-      </fill>
-    </dxf>
     <dxf>
       <font>
         <color rgb="FFFFFFFF"/>
@@ -654,6 +664,14 @@
         <patternFill patternType="solid">
           <fgColor rgb="FFB7E1CD"/>
           <bgColor rgb="FFB7E1CD"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFCC4125"/>
+          <bgColor rgb="FFCC4125"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1164,10 +1182,10 @@
   <dimension ref="A1:T1014"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="M2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="L2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="V16" sqref="V16"/>
+      <selection pane="bottomRight" activeCell="U11" sqref="U11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -1302,12 +1320,11 @@
       <c r="R2" s="6">
         <v>19</v>
       </c>
-      <c r="S2" s="6">
-        <v>19</v>
-      </c>
-      <c r="T2" s="6" t="str">
-        <f t="shared" ref="T2:T64" si="2">IF(S2&lt;=7, "unlikely to be abnormally sleepy.", IF(S2&lt;=9, "average amount of daytime sleepiness.", IF(S2&lt;=15, "may be excessively sleepy", "excessively sleepy.")))</f>
-        <v>excessively sleepy.</v>
+      <c r="S2" s="16">
+        <v>11</v>
+      </c>
+      <c r="T2" s="16" t="s">
+        <v>101</v>
       </c>
     </row>
     <row r="3" spans="1:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -1365,12 +1382,11 @@
       <c r="R3" s="10">
         <v>13</v>
       </c>
-      <c r="S3" s="10">
-        <v>8</v>
-      </c>
-      <c r="T3" s="10" t="str">
-        <f t="shared" si="2"/>
-        <v>average amount of daytime sleepiness.</v>
+      <c r="S3" s="16">
+        <v>0</v>
+      </c>
+      <c r="T3" s="16" t="s">
+        <v>102</v>
       </c>
     </row>
     <row r="4" spans="1:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -1430,12 +1446,11 @@
       <c r="R4" s="6">
         <v>12</v>
       </c>
-      <c r="S4" s="6">
-        <v>8</v>
-      </c>
-      <c r="T4" s="6" t="str">
-        <f t="shared" si="2"/>
-        <v>average amount of daytime sleepiness.</v>
+      <c r="S4" s="16">
+        <v>0</v>
+      </c>
+      <c r="T4" s="16" t="s">
+        <v>102</v>
       </c>
     </row>
     <row r="5" spans="1:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -1495,12 +1510,11 @@
       <c r="R5" s="10">
         <v>15</v>
       </c>
-      <c r="S5" s="10">
-        <v>15</v>
-      </c>
-      <c r="T5" s="10" t="str">
-        <f t="shared" si="2"/>
-        <v>may be excessively sleepy</v>
+      <c r="S5" s="16">
+        <v>7</v>
+      </c>
+      <c r="T5" s="16" t="s">
+        <v>102</v>
       </c>
     </row>
     <row r="6" spans="1:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -1560,12 +1574,11 @@
       <c r="R6" s="6">
         <v>15</v>
       </c>
-      <c r="S6" s="6">
-        <v>17</v>
-      </c>
-      <c r="T6" s="6" t="str">
-        <f t="shared" si="2"/>
-        <v>excessively sleepy.</v>
+      <c r="S6" s="16">
+        <v>9</v>
+      </c>
+      <c r="T6" s="16" t="s">
+        <v>103</v>
       </c>
     </row>
     <row r="7" spans="1:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -1625,12 +1638,11 @@
       <c r="R7" s="10">
         <v>22</v>
       </c>
-      <c r="S7" s="10">
-        <v>25</v>
-      </c>
-      <c r="T7" s="10" t="str">
-        <f t="shared" si="2"/>
-        <v>excessively sleepy.</v>
+      <c r="S7" s="16">
+        <v>17</v>
+      </c>
+      <c r="T7" s="16" t="s">
+        <v>104</v>
       </c>
     </row>
     <row r="8" spans="1:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -1690,12 +1702,11 @@
       <c r="R8" s="6">
         <v>14</v>
       </c>
-      <c r="S8" s="6">
-        <v>19</v>
-      </c>
-      <c r="T8" s="6" t="str">
-        <f t="shared" si="2"/>
-        <v>excessively sleepy.</v>
+      <c r="S8" s="16">
+        <v>11</v>
+      </c>
+      <c r="T8" s="16" t="s">
+        <v>101</v>
       </c>
     </row>
     <row r="9" spans="1:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -1753,12 +1764,11 @@
       <c r="R9" s="10">
         <v>17</v>
       </c>
-      <c r="S9" s="10">
-        <v>12</v>
-      </c>
-      <c r="T9" s="10" t="str">
-        <f t="shared" si="2"/>
-        <v>may be excessively sleepy</v>
+      <c r="S9" s="16">
+        <v>4</v>
+      </c>
+      <c r="T9" s="16" t="s">
+        <v>102</v>
       </c>
     </row>
     <row r="10" spans="1:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -1818,12 +1828,11 @@
       <c r="R10" s="6">
         <v>12</v>
       </c>
-      <c r="S10" s="6">
-        <v>17</v>
-      </c>
-      <c r="T10" s="6" t="str">
-        <f t="shared" si="2"/>
-        <v>excessively sleepy.</v>
+      <c r="S10" s="16">
+        <v>9</v>
+      </c>
+      <c r="T10" s="16" t="s">
+        <v>103</v>
       </c>
     </row>
     <row r="11" spans="1:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -1881,12 +1890,11 @@
       <c r="R11" s="10">
         <v>15</v>
       </c>
-      <c r="S11" s="10">
-        <v>18</v>
-      </c>
-      <c r="T11" s="10" t="str">
-        <f t="shared" si="2"/>
-        <v>excessively sleepy.</v>
+      <c r="S11" s="16">
+        <v>10</v>
+      </c>
+      <c r="T11" s="16" t="s">
+        <v>101</v>
       </c>
     </row>
     <row r="12" spans="1:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -1946,12 +1954,11 @@
       <c r="R12" s="6">
         <v>17</v>
       </c>
-      <c r="S12" s="6">
-        <v>17</v>
-      </c>
-      <c r="T12" s="6" t="str">
-        <f t="shared" si="2"/>
-        <v>excessively sleepy.</v>
+      <c r="S12" s="16">
+        <v>9</v>
+      </c>
+      <c r="T12" s="16" t="s">
+        <v>103</v>
       </c>
     </row>
     <row r="13" spans="1:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -2009,12 +2016,11 @@
       <c r="R13" s="10">
         <v>14</v>
       </c>
-      <c r="S13" s="10">
-        <v>21</v>
-      </c>
-      <c r="T13" s="10" t="str">
-        <f t="shared" si="2"/>
-        <v>excessively sleepy.</v>
+      <c r="S13" s="16">
+        <v>13</v>
+      </c>
+      <c r="T13" s="16" t="s">
+        <v>101</v>
       </c>
     </row>
     <row r="14" spans="1:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -2074,12 +2080,11 @@
       <c r="R14" s="6">
         <v>19</v>
       </c>
-      <c r="S14" s="6">
-        <v>20</v>
-      </c>
-      <c r="T14" s="6" t="str">
-        <f t="shared" si="2"/>
-        <v>excessively sleepy.</v>
+      <c r="S14" s="16">
+        <v>12</v>
+      </c>
+      <c r="T14" s="16" t="s">
+        <v>101</v>
       </c>
     </row>
     <row r="15" spans="1:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -2135,12 +2140,11 @@
       <c r="R15" s="10">
         <v>18</v>
       </c>
-      <c r="S15" s="10">
-        <v>24</v>
-      </c>
-      <c r="T15" s="10" t="str">
-        <f t="shared" si="2"/>
-        <v>excessively sleepy.</v>
+      <c r="S15" s="16">
+        <v>16</v>
+      </c>
+      <c r="T15" s="16" t="s">
+        <v>104</v>
       </c>
     </row>
     <row r="16" spans="1:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -2200,12 +2204,11 @@
       <c r="R16" s="6">
         <v>13</v>
       </c>
-      <c r="S16" s="6">
-        <v>18</v>
-      </c>
-      <c r="T16" s="6" t="str">
-        <f t="shared" si="2"/>
-        <v>excessively sleepy.</v>
+      <c r="S16" s="16">
+        <v>10</v>
+      </c>
+      <c r="T16" s="16" t="s">
+        <v>101</v>
       </c>
     </row>
     <row r="17" spans="1:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -2265,12 +2268,11 @@
       <c r="R17" s="10">
         <v>12</v>
       </c>
-      <c r="S17" s="10">
-        <v>21</v>
-      </c>
-      <c r="T17" s="10" t="str">
-        <f t="shared" si="2"/>
-        <v>excessively sleepy.</v>
+      <c r="S17" s="16">
+        <v>13</v>
+      </c>
+      <c r="T17" s="16" t="s">
+        <v>101</v>
       </c>
     </row>
     <row r="18" spans="1:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -2328,12 +2330,11 @@
       <c r="R18" s="6">
         <v>18</v>
       </c>
-      <c r="S18" s="6">
-        <v>9</v>
-      </c>
-      <c r="T18" s="6" t="str">
-        <f t="shared" si="2"/>
-        <v>average amount of daytime sleepiness.</v>
+      <c r="S18" s="16">
+        <v>1</v>
+      </c>
+      <c r="T18" s="16" t="s">
+        <v>102</v>
       </c>
     </row>
     <row r="19" spans="1:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -2393,12 +2394,11 @@
       <c r="R19" s="10">
         <v>19</v>
       </c>
-      <c r="S19" s="10">
-        <v>16</v>
-      </c>
-      <c r="T19" s="10" t="str">
-        <f t="shared" si="2"/>
-        <v>excessively sleepy.</v>
+      <c r="S19" s="16">
+        <v>8</v>
+      </c>
+      <c r="T19" s="16" t="s">
+        <v>103</v>
       </c>
     </row>
     <row r="20" spans="1:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -2458,12 +2458,11 @@
       <c r="R20" s="6">
         <v>18</v>
       </c>
-      <c r="S20" s="6">
-        <v>10</v>
-      </c>
-      <c r="T20" s="6" t="str">
-        <f t="shared" si="2"/>
-        <v>may be excessively sleepy</v>
+      <c r="S20" s="16">
+        <v>2</v>
+      </c>
+      <c r="T20" s="16" t="s">
+        <v>102</v>
       </c>
     </row>
     <row r="21" spans="1:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -2523,12 +2522,11 @@
       <c r="R21" s="10">
         <v>17</v>
       </c>
-      <c r="S21" s="10">
-        <v>19</v>
-      </c>
-      <c r="T21" s="10" t="str">
-        <f t="shared" si="2"/>
-        <v>excessively sleepy.</v>
+      <c r="S21" s="16">
+        <v>11</v>
+      </c>
+      <c r="T21" s="16" t="s">
+        <v>101</v>
       </c>
     </row>
     <row r="22" spans="1:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -2586,12 +2584,11 @@
       <c r="R22" s="6">
         <v>17</v>
       </c>
-      <c r="S22" s="6">
-        <v>21</v>
-      </c>
-      <c r="T22" s="6" t="str">
-        <f t="shared" si="2"/>
-        <v>excessively sleepy.</v>
+      <c r="S22" s="16">
+        <v>13</v>
+      </c>
+      <c r="T22" s="16" t="s">
+        <v>101</v>
       </c>
     </row>
     <row r="23" spans="1:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -2651,12 +2648,11 @@
       <c r="R23" s="10">
         <v>22</v>
       </c>
-      <c r="S23" s="10">
-        <v>9</v>
-      </c>
-      <c r="T23" s="10" t="str">
-        <f t="shared" si="2"/>
-        <v>average amount of daytime sleepiness.</v>
+      <c r="S23" s="16">
+        <v>1</v>
+      </c>
+      <c r="T23" s="16" t="s">
+        <v>102</v>
       </c>
     </row>
     <row r="24" spans="1:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -2716,12 +2712,11 @@
       <c r="R24" s="6">
         <v>17</v>
       </c>
-      <c r="S24" s="6">
-        <v>19</v>
-      </c>
-      <c r="T24" s="6" t="str">
-        <f t="shared" si="2"/>
-        <v>excessively sleepy.</v>
+      <c r="S24" s="16">
+        <v>11</v>
+      </c>
+      <c r="T24" s="16" t="s">
+        <v>101</v>
       </c>
     </row>
     <row r="25" spans="1:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -2781,12 +2776,11 @@
       <c r="R25" s="10">
         <v>20</v>
       </c>
-      <c r="S25" s="10">
-        <v>21</v>
-      </c>
-      <c r="T25" s="10" t="str">
-        <f t="shared" si="2"/>
-        <v>excessively sleepy.</v>
+      <c r="S25" s="16">
+        <v>13</v>
+      </c>
+      <c r="T25" s="16" t="s">
+        <v>101</v>
       </c>
     </row>
     <row r="26" spans="1:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -2846,12 +2840,11 @@
       <c r="R26" s="6">
         <v>18</v>
       </c>
-      <c r="S26" s="6">
-        <v>15</v>
-      </c>
-      <c r="T26" s="6" t="str">
-        <f t="shared" si="2"/>
-        <v>may be excessively sleepy</v>
+      <c r="S26" s="16">
+        <v>7</v>
+      </c>
+      <c r="T26" s="16" t="s">
+        <v>102</v>
       </c>
     </row>
     <row r="27" spans="1:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -2911,12 +2904,11 @@
       <c r="R27" s="10">
         <v>12</v>
       </c>
-      <c r="S27" s="10">
-        <v>17</v>
-      </c>
-      <c r="T27" s="10" t="str">
-        <f t="shared" si="2"/>
-        <v>excessively sleepy.</v>
+      <c r="S27" s="16">
+        <v>9</v>
+      </c>
+      <c r="T27" s="16" t="s">
+        <v>103</v>
       </c>
     </row>
     <row r="28" spans="1:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -2976,12 +2968,11 @@
       <c r="R28" s="6">
         <v>17</v>
       </c>
-      <c r="S28" s="6">
-        <v>17</v>
-      </c>
-      <c r="T28" s="6" t="str">
-        <f t="shared" si="2"/>
-        <v>excessively sleepy.</v>
+      <c r="S28" s="16">
+        <v>9</v>
+      </c>
+      <c r="T28" s="16" t="s">
+        <v>103</v>
       </c>
     </row>
     <row r="29" spans="1:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -3041,12 +3032,11 @@
       <c r="R29" s="10">
         <v>21</v>
       </c>
-      <c r="S29" s="10">
-        <v>22</v>
-      </c>
-      <c r="T29" s="10" t="str">
-        <f t="shared" si="2"/>
-        <v>excessively sleepy.</v>
+      <c r="S29" s="16">
+        <v>14</v>
+      </c>
+      <c r="T29" s="16" t="s">
+        <v>101</v>
       </c>
     </row>
     <row r="30" spans="1:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -3104,12 +3094,11 @@
       <c r="R30" s="6">
         <v>14</v>
       </c>
-      <c r="S30" s="6">
-        <v>12</v>
-      </c>
-      <c r="T30" s="6" t="str">
-        <f t="shared" si="2"/>
-        <v>may be excessively sleepy</v>
+      <c r="S30" s="16">
+        <v>4</v>
+      </c>
+      <c r="T30" s="16" t="s">
+        <v>102</v>
       </c>
     </row>
     <row r="31" spans="1:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -3167,12 +3156,11 @@
       <c r="R31" s="10">
         <v>17</v>
       </c>
-      <c r="S31" s="10">
-        <v>11</v>
-      </c>
-      <c r="T31" s="10" t="str">
-        <f t="shared" si="2"/>
-        <v>may be excessively sleepy</v>
+      <c r="S31" s="16">
+        <v>3</v>
+      </c>
+      <c r="T31" s="16" t="s">
+        <v>102</v>
       </c>
     </row>
     <row r="32" spans="1:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -3232,12 +3220,11 @@
       <c r="R32" s="6">
         <v>15</v>
       </c>
-      <c r="S32" s="6">
-        <v>18</v>
-      </c>
-      <c r="T32" s="6" t="str">
-        <f t="shared" si="2"/>
-        <v>excessively sleepy.</v>
+      <c r="S32" s="16">
+        <v>10</v>
+      </c>
+      <c r="T32" s="16" t="s">
+        <v>101</v>
       </c>
     </row>
     <row r="33" spans="1:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -3297,12 +3284,11 @@
       <c r="R33" s="10">
         <v>14</v>
       </c>
-      <c r="S33" s="10">
-        <v>19</v>
-      </c>
-      <c r="T33" s="10" t="str">
-        <f t="shared" si="2"/>
-        <v>excessively sleepy.</v>
+      <c r="S33" s="16">
+        <v>11</v>
+      </c>
+      <c r="T33" s="16" t="s">
+        <v>101</v>
       </c>
     </row>
     <row r="34" spans="1:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -3358,12 +3344,11 @@
       <c r="R34" s="6">
         <v>3</v>
       </c>
-      <c r="S34" s="6">
+      <c r="S34" s="16">
         <v>4</v>
       </c>
-      <c r="T34" s="6" t="str">
-        <f t="shared" si="2"/>
-        <v>unlikely to be abnormally sleepy.</v>
+      <c r="T34" s="16" t="s">
+        <v>102</v>
       </c>
     </row>
     <row r="35" spans="1:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -3417,12 +3402,11 @@
       <c r="R35" s="10">
         <v>11</v>
       </c>
-      <c r="S35" s="10">
+      <c r="S35" s="16">
         <v>7</v>
       </c>
-      <c r="T35" s="10" t="str">
-        <f t="shared" si="2"/>
-        <v>unlikely to be abnormally sleepy.</v>
+      <c r="T35" s="16" t="s">
+        <v>102</v>
       </c>
     </row>
     <row r="36" spans="1:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -3476,12 +3460,11 @@
       <c r="R36" s="6">
         <v>10</v>
       </c>
-      <c r="S36" s="6">
+      <c r="S36" s="16">
         <v>12</v>
       </c>
-      <c r="T36" s="6" t="str">
-        <f t="shared" si="2"/>
-        <v>may be excessively sleepy</v>
+      <c r="T36" s="16" t="s">
+        <v>101</v>
       </c>
     </row>
     <row r="37" spans="1:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -3535,12 +3518,11 @@
       <c r="R37" s="10">
         <v>13</v>
       </c>
-      <c r="S37" s="10">
+      <c r="S37" s="16">
         <v>4</v>
       </c>
-      <c r="T37" s="10" t="str">
-        <f t="shared" si="2"/>
-        <v>unlikely to be abnormally sleepy.</v>
+      <c r="T37" s="16" t="s">
+        <v>102</v>
       </c>
     </row>
     <row r="38" spans="1:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -3594,12 +3576,11 @@
       <c r="R38" s="6">
         <v>1</v>
       </c>
-      <c r="S38" s="6">
+      <c r="S38" s="16">
         <v>1</v>
       </c>
-      <c r="T38" s="6" t="str">
-        <f t="shared" si="2"/>
-        <v>unlikely to be abnormally sleepy.</v>
+      <c r="T38" s="16" t="s">
+        <v>102</v>
       </c>
     </row>
     <row r="39" spans="1:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -3653,12 +3634,11 @@
       <c r="R39" s="10">
         <v>3</v>
       </c>
-      <c r="S39" s="10">
+      <c r="S39" s="16">
         <v>9</v>
       </c>
-      <c r="T39" s="10" t="str">
-        <f t="shared" si="2"/>
-        <v>average amount of daytime sleepiness.</v>
+      <c r="T39" s="16" t="s">
+        <v>103</v>
       </c>
     </row>
     <row r="40" spans="1:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -3714,12 +3694,11 @@
       <c r="R40" s="6">
         <v>1</v>
       </c>
-      <c r="S40" s="6">
+      <c r="S40" s="16">
         <v>9</v>
       </c>
-      <c r="T40" s="6" t="str">
-        <f t="shared" si="2"/>
-        <v>average amount of daytime sleepiness.</v>
+      <c r="T40" s="16" t="s">
+        <v>103</v>
       </c>
     </row>
     <row r="41" spans="1:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -3773,12 +3752,11 @@
       <c r="R41" s="10">
         <v>13</v>
       </c>
-      <c r="S41" s="10">
+      <c r="S41" s="16">
         <v>2</v>
       </c>
-      <c r="T41" s="10" t="str">
-        <f t="shared" si="2"/>
-        <v>unlikely to be abnormally sleepy.</v>
+      <c r="T41" s="16" t="s">
+        <v>102</v>
       </c>
     </row>
     <row r="42" spans="1:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -3832,12 +3810,11 @@
       <c r="R42" s="6">
         <v>12</v>
       </c>
-      <c r="S42" s="6">
+      <c r="S42" s="16">
         <v>7</v>
       </c>
-      <c r="T42" s="6" t="str">
-        <f t="shared" si="2"/>
-        <v>unlikely to be abnormally sleepy.</v>
+      <c r="T42" s="16" t="s">
+        <v>102</v>
       </c>
     </row>
     <row r="43" spans="1:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -3891,12 +3868,11 @@
       <c r="R43" s="10">
         <v>13</v>
       </c>
-      <c r="S43" s="10">
+      <c r="S43" s="16">
         <v>9</v>
       </c>
-      <c r="T43" s="10" t="str">
-        <f t="shared" si="2"/>
-        <v>average amount of daytime sleepiness.</v>
+      <c r="T43" s="16" t="s">
+        <v>103</v>
       </c>
     </row>
     <row r="44" spans="1:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -3950,12 +3926,11 @@
       <c r="R44" s="6">
         <v>5</v>
       </c>
-      <c r="S44" s="6">
+      <c r="S44" s="16">
         <v>6</v>
       </c>
-      <c r="T44" s="6" t="str">
-        <f t="shared" si="2"/>
-        <v>unlikely to be abnormally sleepy.</v>
+      <c r="T44" s="16" t="s">
+        <v>102</v>
       </c>
     </row>
     <row r="45" spans="1:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -4009,12 +3984,11 @@
       <c r="R45" s="10">
         <v>5</v>
       </c>
-      <c r="S45" s="10">
+      <c r="S45" s="16">
         <v>2</v>
       </c>
-      <c r="T45" s="10" t="str">
-        <f t="shared" si="2"/>
-        <v>unlikely to be abnormally sleepy.</v>
+      <c r="T45" s="16" t="s">
+        <v>102</v>
       </c>
     </row>
     <row r="46" spans="1:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -4068,12 +4042,11 @@
       <c r="R46" s="6">
         <v>14</v>
       </c>
-      <c r="S46" s="6">
+      <c r="S46" s="16">
         <v>10</v>
       </c>
-      <c r="T46" s="6" t="str">
-        <f t="shared" si="2"/>
-        <v>may be excessively sleepy</v>
+      <c r="T46" s="16" t="s">
+        <v>101</v>
       </c>
     </row>
     <row r="47" spans="1:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -4127,12 +4100,11 @@
       <c r="R47" s="10">
         <v>6</v>
       </c>
-      <c r="S47" s="10">
+      <c r="S47" s="16">
         <v>8</v>
       </c>
-      <c r="T47" s="10" t="str">
-        <f t="shared" si="2"/>
-        <v>average amount of daytime sleepiness.</v>
+      <c r="T47" s="16" t="s">
+        <v>103</v>
       </c>
     </row>
     <row r="48" spans="1:20" ht="13" x14ac:dyDescent="0.15">
@@ -4186,12 +4158,11 @@
       <c r="R48" s="6">
         <v>16</v>
       </c>
-      <c r="S48" s="6">
+      <c r="S48" s="16">
         <v>9</v>
       </c>
-      <c r="T48" s="6" t="str">
-        <f t="shared" si="2"/>
-        <v>average amount of daytime sleepiness.</v>
+      <c r="T48" s="16" t="s">
+        <v>103</v>
       </c>
     </row>
     <row r="49" spans="1:20" ht="13" x14ac:dyDescent="0.15">
@@ -4245,12 +4216,11 @@
       <c r="R49" s="10">
         <v>5</v>
       </c>
-      <c r="S49" s="10">
+      <c r="S49" s="16">
         <v>7</v>
       </c>
-      <c r="T49" s="10" t="str">
-        <f t="shared" si="2"/>
-        <v>unlikely to be abnormally sleepy.</v>
+      <c r="T49" s="16" t="s">
+        <v>102</v>
       </c>
     </row>
     <row r="50" spans="1:20" ht="13" x14ac:dyDescent="0.15">
@@ -4304,12 +4274,11 @@
       <c r="R50" s="6">
         <v>9</v>
       </c>
-      <c r="S50" s="6">
+      <c r="S50" s="16">
         <v>11</v>
       </c>
-      <c r="T50" s="6" t="str">
-        <f t="shared" si="2"/>
-        <v>may be excessively sleepy</v>
+      <c r="T50" s="16" t="s">
+        <v>101</v>
       </c>
     </row>
     <row r="51" spans="1:20" ht="13" x14ac:dyDescent="0.15">
@@ -4363,12 +4332,11 @@
       <c r="R51" s="10">
         <v>8</v>
       </c>
-      <c r="S51" s="10">
+      <c r="S51" s="16">
         <v>4</v>
       </c>
-      <c r="T51" s="10" t="str">
-        <f t="shared" si="2"/>
-        <v>unlikely to be abnormally sleepy.</v>
+      <c r="T51" s="16" t="s">
+        <v>102</v>
       </c>
     </row>
     <row r="52" spans="1:20" ht="13" x14ac:dyDescent="0.15">
@@ -4422,12 +4390,11 @@
       <c r="R52" s="6">
         <v>8</v>
       </c>
-      <c r="S52" s="6">
+      <c r="S52" s="16">
         <v>13</v>
       </c>
-      <c r="T52" s="6" t="str">
-        <f t="shared" si="2"/>
-        <v>may be excessively sleepy</v>
+      <c r="T52" s="16" t="s">
+        <v>101</v>
       </c>
     </row>
     <row r="53" spans="1:20" ht="13" x14ac:dyDescent="0.15">
@@ -4481,12 +4448,11 @@
       <c r="R53" s="10">
         <v>8</v>
       </c>
-      <c r="S53" s="10">
+      <c r="S53" s="16">
         <v>1</v>
       </c>
-      <c r="T53" s="10" t="str">
-        <f t="shared" si="2"/>
-        <v>unlikely to be abnormally sleepy.</v>
+      <c r="T53" s="16" t="s">
+        <v>102</v>
       </c>
     </row>
     <row r="54" spans="1:20" ht="13" x14ac:dyDescent="0.15">
@@ -4540,12 +4506,11 @@
       <c r="R54" s="6">
         <v>8</v>
       </c>
-      <c r="S54" s="6">
+      <c r="S54" s="16">
         <v>4</v>
       </c>
-      <c r="T54" s="6" t="str">
-        <f t="shared" si="2"/>
-        <v>unlikely to be abnormally sleepy.</v>
+      <c r="T54" s="16" t="s">
+        <v>102</v>
       </c>
     </row>
     <row r="55" spans="1:20" ht="13" x14ac:dyDescent="0.15">
@@ -4599,12 +4564,11 @@
       <c r="R55" s="10">
         <v>9</v>
       </c>
-      <c r="S55" s="10">
+      <c r="S55" s="16">
         <v>13</v>
       </c>
-      <c r="T55" s="10" t="str">
-        <f t="shared" si="2"/>
-        <v>may be excessively sleepy</v>
+      <c r="T55" s="16" t="s">
+        <v>101</v>
       </c>
     </row>
     <row r="56" spans="1:20" ht="13" x14ac:dyDescent="0.15">
@@ -4658,12 +4622,11 @@
       <c r="R56" s="6">
         <v>10</v>
       </c>
-      <c r="S56" s="6">
+      <c r="S56" s="16">
         <v>10</v>
       </c>
-      <c r="T56" s="6" t="str">
-        <f t="shared" si="2"/>
-        <v>may be excessively sleepy</v>
+      <c r="T56" s="16" t="s">
+        <v>101</v>
       </c>
     </row>
     <row r="57" spans="1:20" ht="13" x14ac:dyDescent="0.15">
@@ -4717,12 +4680,11 @@
       <c r="R57" s="10">
         <v>4</v>
       </c>
-      <c r="S57" s="10">
+      <c r="S57" s="16">
         <v>5</v>
       </c>
-      <c r="T57" s="10" t="str">
-        <f t="shared" si="2"/>
-        <v>unlikely to be abnormally sleepy.</v>
+      <c r="T57" s="16" t="s">
+        <v>102</v>
       </c>
     </row>
     <row r="58" spans="1:20" ht="13" x14ac:dyDescent="0.15">
@@ -4776,12 +4738,11 @@
       <c r="R58" s="6">
         <v>7</v>
       </c>
-      <c r="S58" s="6">
+      <c r="S58" s="16">
         <v>8</v>
       </c>
-      <c r="T58" s="6" t="str">
-        <f t="shared" si="2"/>
-        <v>average amount of daytime sleepiness.</v>
+      <c r="T58" s="16" t="s">
+        <v>103</v>
       </c>
     </row>
     <row r="59" spans="1:20" ht="13" x14ac:dyDescent="0.15">
@@ -4835,12 +4796,11 @@
       <c r="R59" s="10">
         <v>6</v>
       </c>
-      <c r="S59" s="10">
+      <c r="S59" s="16">
         <v>8</v>
       </c>
-      <c r="T59" s="10" t="str">
-        <f t="shared" si="2"/>
-        <v>average amount of daytime sleepiness.</v>
+      <c r="T59" s="16" t="s">
+        <v>103</v>
       </c>
     </row>
     <row r="60" spans="1:20" ht="13" x14ac:dyDescent="0.15">
@@ -4894,12 +4854,11 @@
       <c r="R60" s="6">
         <v>2</v>
       </c>
-      <c r="S60" s="6">
+      <c r="S60" s="16">
         <v>2</v>
       </c>
-      <c r="T60" s="6" t="str">
-        <f t="shared" si="2"/>
-        <v>unlikely to be abnormally sleepy.</v>
+      <c r="T60" s="16" t="s">
+        <v>102</v>
       </c>
     </row>
     <row r="61" spans="1:20" ht="13" x14ac:dyDescent="0.15">
@@ -4953,12 +4912,11 @@
       <c r="R61" s="10">
         <v>12</v>
       </c>
-      <c r="S61" s="10">
+      <c r="S61" s="16">
         <v>10</v>
       </c>
-      <c r="T61" s="10" t="str">
-        <f t="shared" si="2"/>
-        <v>may be excessively sleepy</v>
+      <c r="T61" s="16" t="s">
+        <v>101</v>
       </c>
     </row>
     <row r="62" spans="1:20" ht="13" x14ac:dyDescent="0.15">
@@ -5012,12 +4970,11 @@
       <c r="R62" s="6">
         <v>9</v>
       </c>
-      <c r="S62" s="6">
+      <c r="S62" s="16">
         <v>3</v>
       </c>
-      <c r="T62" s="6" t="str">
-        <f t="shared" si="2"/>
-        <v>unlikely to be abnormally sleepy.</v>
+      <c r="T62" s="16" t="s">
+        <v>102</v>
       </c>
     </row>
     <row r="63" spans="1:20" ht="13" x14ac:dyDescent="0.15">
@@ -5071,12 +5028,11 @@
       <c r="R63" s="10">
         <v>2</v>
       </c>
-      <c r="S63" s="10">
+      <c r="S63" s="16">
         <v>6</v>
       </c>
-      <c r="T63" s="10" t="str">
-        <f t="shared" si="2"/>
-        <v>unlikely to be abnormally sleepy.</v>
+      <c r="T63" s="16" t="s">
+        <v>102</v>
       </c>
     </row>
     <row r="64" spans="1:20" ht="13" x14ac:dyDescent="0.15">
@@ -5130,12 +5086,11 @@
       <c r="R64" s="6">
         <v>10</v>
       </c>
-      <c r="S64" s="6">
+      <c r="S64" s="16">
         <v>11</v>
       </c>
-      <c r="T64" s="6" t="str">
-        <f t="shared" si="2"/>
-        <v>may be excessively sleepy</v>
+      <c r="T64" s="16" t="s">
+        <v>101</v>
       </c>
     </row>
     <row r="65" spans="1:20" ht="13" x14ac:dyDescent="0.15">
@@ -26039,34 +25994,17 @@
       <c r="T1014" s="14"/>
     </row>
   </sheetData>
+  <conditionalFormatting sqref="A65:T998 A2:R64">
+    <cfRule type="expression" dxfId="7" priority="9">
+      <formula>#REF!=TRUE</formula>
+    </cfRule>
+  </conditionalFormatting>
   <conditionalFormatting sqref="I2:J33">
-    <cfRule type="expression" dxfId="7" priority="1">
+    <cfRule type="expression" dxfId="6" priority="1">
       <formula>$I2=$J2</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="6" priority="8">
+    <cfRule type="expression" dxfId="5" priority="8">
       <formula>$I2&lt;&gt;$J2</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="T2:T64">
-    <cfRule type="expression" dxfId="5" priority="2">
-      <formula>$P2=TRUE</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="4" priority="3">
-      <formula>$N2="unlikely to be abnormally sleepy."</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="3" priority="4">
-      <formula>$N2="average amount of daytime sleepiness."</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="2" priority="5">
-      <formula>$N2="may be excessively sleepy"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="1" priority="6">
-      <formula>$N2="excessively sleepy."</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A2:T998">
-    <cfRule type="expression" dxfId="0" priority="9">
-      <formula>#REF!=TRUE</formula>
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="6">

</xml_diff>